<commit_message>
Revu le calcul transtion, le donjon puzzle et le DDL
</commit_message>
<xml_diff>
--- a/assets/map/CalculsTransitionsDébut2018.xlsx
+++ b/assets/map/CalculsTransitionsDébut2018.xlsx
@@ -1,22 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tallentaa\assets\map\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634DD053-2BF2-4C98-A738-064EBA4A6127}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="27360" windowHeight="12525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10575" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1 - 18 bits" sheetId="1" r:id="rId1"/>
-    <sheet name="v1 - 15 bits" sheetId="4" r:id="rId2"/>
+    <sheet name="v2 - 15 bits" sheetId="4" r:id="rId2"/>
     <sheet name="Feuil5" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Damien Gouteux</author>
+  </authors>
+  <commentList>
+    <comment ref="AF2" authorId="0" shapeId="0" xr:uid="{63A460C9-5982-43E7-B132-45A4BEC45986}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Damien Gouteux:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+border
+or
+corner</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="51">
   <si>
     <t>rien</t>
   </si>
@@ -134,12 +176,48 @@
   <si>
     <t>to_sand</t>
   </si>
+  <si>
+    <t>Principe</t>
+  </si>
+  <si>
+    <t>Le principe est simple :</t>
+  </si>
+  <si>
+    <t>5 bits pour  coder les transitions = 1 bit pour identifier coin ou bord puis 1 bit / possibilité.</t>
+  </si>
+  <si>
+    <t>5 bits pour coder le premier type vers lequel on transite</t>
+  </si>
+  <si>
+    <t>5 bits pour coder le second type vers lequel on transite</t>
+  </si>
+  <si>
+    <t>On a donc 2**5 = 32 types possibles.</t>
+  </si>
+  <si>
+    <t>Cela a fonctionné en janvier 2018.</t>
+  </si>
+  <si>
+    <t>La limitation est qu'on peut faire une transition entre 2 types seulement.</t>
+  </si>
+  <si>
+    <t>Type texture</t>
+  </si>
+  <si>
+    <t>Transition</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cette seconde version ne prend que 15 bits, inférieur à ce qu'il faut pour coder un entier en C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,8 +251,27 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,8 +356,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -305,11 +426,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,9 +525,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,6 +544,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,6 +574,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -481,7 +625,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -514,9 +658,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -549,6 +710,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -724,7 +902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -746,23 +924,23 @@
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="31"/>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
       <c r="O1" s="30"/>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="32" t="s">
         <v>23</v>
       </c>
       <c r="Q1" s="31"/>
@@ -2323,7 +2501,7 @@
         <v>8192</v>
       </c>
       <c r="AP14">
-        <f t="shared" ref="AP14:AP24" si="0">AP13*2</f>
+        <f t="shared" ref="AP14:AP18" si="0">AP13*2</f>
         <v>8192</v>
       </c>
       <c r="AQ14" s="1">
@@ -4514,11 +4692,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AQ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4536,73 +4714,73 @@
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="31"/>
-      <c r="B1" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="33"/>
+      <c r="B1" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
       <c r="R1" s="30"/>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="32" t="s">
         <v>23</v>
       </c>
       <c r="T1" s="31"/>
       <c r="U1" s="31"/>
-      <c r="V1" s="39">
-        <v>0</v>
-      </c>
-      <c r="W1" s="39">
-        <v>0</v>
-      </c>
-      <c r="X1" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y1" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AA1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AB1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AC1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AF1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AG1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AH1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI1" s="39">
-        <v>0</v>
-      </c>
-      <c r="AJ1" s="39">
+      <c r="V1" s="38">
+        <v>0</v>
+      </c>
+      <c r="W1" s="38">
+        <v>0</v>
+      </c>
+      <c r="X1" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AF1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AG1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AH1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AI1" s="38">
+        <v>0</v>
+      </c>
+      <c r="AJ1" s="38">
         <v>0</v>
       </c>
       <c r="AN1" t="s">
@@ -4623,78 +4801,36 @@
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="28">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="R2" s="30"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="35" t="s">
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="AG2" s="35" t="s">
+      <c r="AG2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="AH2" s="35" t="s">
+      <c r="AH2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="AI2" s="35" t="s">
+      <c r="AI2" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="AJ2" s="35" t="s">
+      <c r="AJ2" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="AK2" s="35" t="s">
+      <c r="AK2" s="34" t="s">
         <v>34</v>
       </c>
       <c r="AO2">
@@ -4712,49 +4848,7 @@
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>1</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="28">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="R3" s="30"/>
       <c r="S3" s="27">
@@ -4791,7 +4885,7 @@
       <c r="AD3" s="16">
         <v>0</v>
       </c>
-      <c r="AE3" s="37">
+      <c r="AE3" s="36">
         <v>0</v>
       </c>
       <c r="AF3" s="13">
@@ -4809,7 +4903,7 @@
       <c r="AJ3" s="13">
         <v>0</v>
       </c>
-      <c r="AK3" s="40">
+      <c r="AK3" s="39">
         <v>1</v>
       </c>
       <c r="AN3" t="s">
@@ -4830,49 +4924,7 @@
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="28">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="R4" s="30"/>
       <c r="S4" s="27">
@@ -4927,7 +4979,7 @@
       <c r="AJ4" s="13">
         <v>0</v>
       </c>
-      <c r="AK4" s="40">
+      <c r="AK4" s="39">
         <v>2</v>
       </c>
       <c r="AN4" t="s">
@@ -4948,49 +5000,7 @@
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="28">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="R5" s="31"/>
       <c r="S5" s="27">
@@ -5045,7 +5055,7 @@
       <c r="AJ5" s="13">
         <v>0</v>
       </c>
-      <c r="AK5" s="40">
+      <c r="AK5" s="39">
         <v>3</v>
       </c>
       <c r="AO5">
@@ -5063,25 +5073,7 @@
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="R6" s="30"/>
       <c r="S6" s="27">
@@ -5091,7 +5083,7 @@
         <v>10</v>
       </c>
       <c r="U6" s="24"/>
-      <c r="V6" s="36">
+      <c r="V6" s="35">
         <v>0</v>
       </c>
       <c r="W6" s="22">
@@ -5118,7 +5110,7 @@
       <c r="AD6" s="22">
         <v>0</v>
       </c>
-      <c r="AE6" s="38">
+      <c r="AE6" s="37">
         <v>0</v>
       </c>
       <c r="AF6" s="13">
@@ -5136,7 +5128,7 @@
       <c r="AJ6" s="13">
         <v>0</v>
       </c>
-      <c r="AK6" s="40">
+      <c r="AK6" s="39">
         <v>4</v>
       </c>
       <c r="AO6">
@@ -5154,61 +5146,19 @@
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="28">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="R7" s="30"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="34"/>
-      <c r="AC7" s="34"/>
-      <c r="AD7" s="34"/>
-      <c r="AE7" s="34"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
+      <c r="AA7" s="33"/>
+      <c r="AB7" s="33"/>
+      <c r="AC7" s="33"/>
+      <c r="AD7" s="33"/>
+      <c r="AE7" s="33"/>
       <c r="AF7" s="21"/>
       <c r="AG7" s="21"/>
       <c r="AH7" s="21"/>
@@ -5229,49 +5179,7 @@
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
-        <v>1</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="28">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="R8" s="30"/>
       <c r="S8" s="27">
@@ -5325,7 +5233,7 @@
       <c r="AJ8" s="21">
         <v>0</v>
       </c>
-      <c r="AK8" s="40">
+      <c r="AK8" s="39">
         <v>1</v>
       </c>
       <c r="AO8">
@@ -5343,49 +5251,7 @@
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="2">
-        <v>1</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <v>1</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="28">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="R9" s="30"/>
       <c r="S9" s="27">
@@ -5439,7 +5305,7 @@
       <c r="AJ9" s="21">
         <v>0</v>
       </c>
-      <c r="AK9" s="40">
+      <c r="AK9" s="39">
         <v>2</v>
       </c>
       <c r="AO9">
@@ -5456,51 +5322,6 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1</v>
-      </c>
-      <c r="M10" s="2">
-        <v>1</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="28">
-        <v>24</v>
-      </c>
       <c r="R10" s="31"/>
       <c r="S10" s="27">
         <v>96</v>
@@ -5553,7 +5374,7 @@
       <c r="AJ10" s="21">
         <v>0</v>
       </c>
-      <c r="AK10" s="40">
+      <c r="AK10" s="39">
         <v>3</v>
       </c>
       <c r="AO10">
@@ -5570,36 +5391,24 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
+      <c r="B11" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="32"/>
       <c r="R11" s="31"/>
       <c r="S11" s="27">
         <v>128</v>
@@ -5652,7 +5461,7 @@
       <c r="AJ11" s="21">
         <v>0</v>
       </c>
-      <c r="AK11" s="40">
+      <c r="AK11" s="39">
         <v>4</v>
       </c>
       <c r="AO11">
@@ -5669,40 +5478,37 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="B12" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
       <c r="R12" s="31"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="34"/>
-      <c r="Z12" s="34"/>
-      <c r="AA12" s="34"/>
-      <c r="AB12" s="34"/>
-      <c r="AC12" s="34"/>
-      <c r="AD12" s="34"/>
-      <c r="AE12" s="34"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="33"/>
+      <c r="Y12" s="33"/>
+      <c r="Z12" s="33"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="33"/>
+      <c r="AE12" s="33"/>
       <c r="AF12" s="21"/>
       <c r="AG12" s="21"/>
       <c r="AH12" s="21"/>
@@ -5722,40 +5528,63 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+      <c r="B13" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="44">
+        <v>0</v>
+      </c>
+      <c r="E13" s="44">
+        <v>0</v>
+      </c>
+      <c r="F13" s="44">
+        <v>0</v>
+      </c>
+      <c r="G13" s="44">
+        <v>0</v>
+      </c>
+      <c r="H13" s="44">
+        <v>0</v>
+      </c>
+      <c r="I13" s="45"/>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="28">
+        <v>1</v>
+      </c>
       <c r="R13" s="31"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
-      <c r="AA13" s="34"/>
-      <c r="AB13" s="34"/>
-      <c r="AC13" s="34"/>
-      <c r="AD13" s="34"/>
-      <c r="AE13" s="34"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="33"/>
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33"/>
+      <c r="AE13" s="33"/>
       <c r="AF13" s="21"/>
       <c r="AG13" s="21"/>
       <c r="AH13" s="21"/>
@@ -5776,28 +5605,51 @@
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="45"/>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="28">
+        <v>2</v>
+      </c>
       <c r="R14" s="31"/>
       <c r="S14" s="28">
         <v>1089</v>
@@ -5873,29 +5725,52 @@
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
+      <c r="B15" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="44">
+        <v>0</v>
+      </c>
+      <c r="E15" s="44">
+        <v>0</v>
+      </c>
+      <c r="F15" s="44">
+        <v>0</v>
+      </c>
+      <c r="G15" s="44">
+        <v>1</v>
+      </c>
+      <c r="H15" s="44">
+        <v>0</v>
+      </c>
+      <c r="I15" s="45"/>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="28">
+        <v>4</v>
+      </c>
       <c r="R15" s="31"/>
       <c r="S15" s="28">
         <v>1090</v>
@@ -5972,28 +5847,51 @@
     <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
         <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="45"/>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="28">
+        <v>8</v>
+      </c>
       <c r="R16" s="31"/>
       <c r="S16" s="28">
         <v>1092</v>
@@ -6065,29 +5963,28 @@
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2">
-        <v>1</v>
-      </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
+      <c r="B17" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="44">
+        <v>0</v>
+      </c>
+      <c r="E17" s="44">
+        <v>0</v>
+      </c>
+      <c r="F17" s="44">
+        <v>1</v>
+      </c>
+      <c r="G17" s="44">
+        <v>0</v>
+      </c>
+      <c r="H17" s="44">
+        <v>0</v>
+      </c>
+      <c r="I17" s="45"/>
       <c r="R17" s="31"/>
       <c r="S17" s="28">
         <v>1096</v>
@@ -6159,22 +6056,45 @@
         <v>5</v>
       </c>
       <c r="D18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
+        <v>1</v>
+      </c>
+      <c r="I18" s="45"/>
+      <c r="J18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="28">
+        <v>17</v>
+      </c>
       <c r="R18" s="31"/>
       <c r="S18" s="28">
         <v>1097</v>
@@ -6242,29 +6162,52 @@
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
-      <c r="B19" t="s">
+      <c r="B19" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="2">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="D19" s="44">
+        <v>0</v>
+      </c>
+      <c r="E19" s="44">
+        <v>0</v>
+      </c>
+      <c r="F19" s="44">
+        <v>1</v>
+      </c>
+      <c r="G19" s="44">
+        <v>1</v>
+      </c>
+      <c r="H19" s="44">
+        <v>0</v>
+      </c>
+      <c r="I19" s="45"/>
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="28">
+        <v>18</v>
+      </c>
       <c r="R19" s="31"/>
       <c r="S19" s="28">
         <v>1091</v>
@@ -6339,22 +6282,45 @@
         <v>5</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2">
         <v>1</v>
       </c>
       <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="45"/>
+      <c r="J20" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="28">
+        <v>20</v>
+      </c>
       <c r="R20" s="31"/>
       <c r="S20" s="28">
         <v>1094</v>
@@ -6422,29 +6388,52 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
-      <c r="B21" t="s">
+      <c r="B21" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="2">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
+      <c r="D21" s="44">
+        <v>0</v>
+      </c>
+      <c r="E21" s="44">
+        <v>1</v>
+      </c>
+      <c r="F21" s="44">
+        <v>0</v>
+      </c>
+      <c r="G21" s="44">
+        <v>0</v>
+      </c>
+      <c r="H21" s="44">
+        <v>0</v>
+      </c>
+      <c r="I21" s="45"/>
+      <c r="J21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="28">
+        <v>24</v>
+      </c>
       <c r="R21" s="31"/>
       <c r="S21" s="28">
         <v>1100</v>
@@ -6519,22 +6508,29 @@
         <v>5</v>
       </c>
       <c r="D22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
       </c>
       <c r="H22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
       <c r="R22" s="31"/>
       <c r="S22" s="28">
         <v>1105</v>
@@ -6599,26 +6595,26 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
-      <c r="B23" t="s">
+      <c r="B23" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="2">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1</v>
+      <c r="D23" s="44">
+        <v>0</v>
+      </c>
+      <c r="E23" s="44">
+        <v>1</v>
+      </c>
+      <c r="F23" s="44">
+        <v>0</v>
+      </c>
+      <c r="G23" s="44">
+        <v>1</v>
+      </c>
+      <c r="H23" s="44">
+        <v>0</v>
       </c>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
@@ -6693,19 +6689,19 @@
         <v>5</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2">
         <v>1</v>
       </c>
       <c r="H24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
@@ -6773,26 +6769,26 @@
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
-      <c r="B25" t="s">
+      <c r="B25" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="2">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
-      <c r="H25" s="2">
-        <v>1</v>
+      <c r="D25" s="44">
+        <v>0</v>
+      </c>
+      <c r="E25" s="44">
+        <v>1</v>
+      </c>
+      <c r="F25" s="44">
+        <v>1</v>
+      </c>
+      <c r="G25" s="44">
+        <v>0</v>
+      </c>
+      <c r="H25" s="44">
+        <v>0</v>
       </c>
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
@@ -6867,19 +6863,19 @@
         <v>5</v>
       </c>
       <c r="D26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
       </c>
       <c r="F26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="2">
         <v>0</v>
       </c>
       <c r="H26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="31"/>
       <c r="J26" s="31"/>
@@ -6947,26 +6943,26 @@
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
-      <c r="B27" t="s">
+      <c r="B27" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1</v>
+      <c r="D27" s="44">
+        <v>0</v>
+      </c>
+      <c r="E27" s="44">
+        <v>1</v>
+      </c>
+      <c r="F27" s="44">
+        <v>1</v>
+      </c>
+      <c r="G27" s="44">
+        <v>1</v>
+      </c>
+      <c r="H27" s="44">
+        <v>0</v>
       </c>
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
@@ -7041,19 +7037,19 @@
         <v>5</v>
       </c>
       <c r="D28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
       </c>
       <c r="F28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="2">
         <v>1</v>
       </c>
       <c r="H28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -7121,26 +7117,26 @@
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
-      <c r="B29" t="s">
+      <c r="B29" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1</v>
+      <c r="D29" s="44">
+        <v>1</v>
+      </c>
+      <c r="E29" s="44">
+        <v>0</v>
+      </c>
+      <c r="F29" s="44">
+        <v>0</v>
+      </c>
+      <c r="G29" s="44">
+        <v>0</v>
+      </c>
+      <c r="H29" s="44">
+        <v>0</v>
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
@@ -7218,16 +7214,16 @@
         <v>1</v>
       </c>
       <c r="E30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
       </c>
       <c r="H30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="31"/>
       <c r="J30" s="31"/>
@@ -7298,26 +7294,26 @@
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
-      <c r="B31" t="s">
+      <c r="B31" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="2">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1</v>
+      <c r="D31" s="44">
+        <v>1</v>
+      </c>
+      <c r="E31" s="44">
+        <v>0</v>
+      </c>
+      <c r="F31" s="44">
+        <v>0</v>
+      </c>
+      <c r="G31" s="44">
+        <v>1</v>
+      </c>
+      <c r="H31" s="44">
+        <v>0</v>
       </c>
       <c r="I31" s="31"/>
       <c r="J31" s="31"/>
@@ -7398,16 +7394,16 @@
         <v>1</v>
       </c>
       <c r="E32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="2">
         <v>1</v>
       </c>
       <c r="H32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="31"/>
       <c r="J32" s="31"/>
@@ -7478,26 +7474,26 @@
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
-      <c r="B33" t="s">
+      <c r="B33" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2">
-        <v>1</v>
-      </c>
-      <c r="H33" s="2">
-        <v>1</v>
+      <c r="D33" s="44">
+        <v>1</v>
+      </c>
+      <c r="E33" s="44">
+        <v>0</v>
+      </c>
+      <c r="F33" s="44">
+        <v>1</v>
+      </c>
+      <c r="G33" s="44">
+        <v>0</v>
+      </c>
+      <c r="H33" s="44">
+        <v>0</v>
       </c>
       <c r="I33" s="31"/>
       <c r="J33" s="31"/>
@@ -7568,13 +7564,27 @@
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1</v>
+      </c>
       <c r="I34" s="31"/>
       <c r="J34" s="31"/>
       <c r="R34" s="31"/>
@@ -7640,6 +7650,30 @@
       </c>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
+      <c r="B35" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="44">
+        <v>1</v>
+      </c>
+      <c r="E35" s="44">
+        <v>0</v>
+      </c>
+      <c r="F35" s="44">
+        <v>1</v>
+      </c>
+      <c r="G35" s="44">
+        <v>1</v>
+      </c>
+      <c r="H35" s="44">
+        <v>0</v>
+      </c>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
       <c r="R35" s="31"/>
       <c r="S35" s="28">
         <v>2162</v>
@@ -7703,6 +7737,30 @@
       </c>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1</v>
+      </c>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
       <c r="R36" s="31"/>
       <c r="S36" s="28">
         <v>2164</v>
@@ -7766,6 +7824,30 @@
       </c>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
+      <c r="B37" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="44">
+        <v>1</v>
+      </c>
+      <c r="E37" s="44">
+        <v>1</v>
+      </c>
+      <c r="F37" s="44">
+        <v>0</v>
+      </c>
+      <c r="G37" s="44">
+        <v>0</v>
+      </c>
+      <c r="H37" s="44">
+        <v>0</v>
+      </c>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
       <c r="R37" s="31"/>
       <c r="S37" s="28">
         <v>2168</v>
@@ -7829,6 +7911,30 @@
       </c>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38" s="31"/>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>1</v>
+      </c>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
       <c r="R38" s="31"/>
       <c r="S38" s="28">
         <v>1153</v>
@@ -7892,6 +7998,30 @@
       </c>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
+      <c r="B39" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="44">
+        <v>1</v>
+      </c>
+      <c r="E39" s="44">
+        <v>1</v>
+      </c>
+      <c r="F39" s="44">
+        <v>0</v>
+      </c>
+      <c r="G39" s="44">
+        <v>1</v>
+      </c>
+      <c r="H39" s="44">
+        <v>0</v>
+      </c>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
       <c r="R39" s="31"/>
       <c r="S39" s="28">
         <v>1154</v>
@@ -7955,6 +8085,30 @@
       </c>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1</v>
+      </c>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
       <c r="R40" s="31"/>
       <c r="S40" s="28">
         <v>1156</v>
@@ -8018,6 +8172,33 @@
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
+      <c r="B41" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="44">
+        <v>1</v>
+      </c>
+      <c r="E41" s="44">
+        <v>1</v>
+      </c>
+      <c r="F41" s="44">
+        <v>1</v>
+      </c>
+      <c r="G41" s="44">
+        <v>0</v>
+      </c>
+      <c r="H41" s="44">
+        <v>0</v>
+      </c>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="N41" t="s">
+        <v>49</v>
+      </c>
       <c r="R41" s="31"/>
       <c r="S41" s="28">
         <v>1160</v>
@@ -8081,6 +8262,30 @@
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1</v>
+      </c>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
       <c r="R42" s="31"/>
       <c r="S42" s="28">
         <v>1161</v>
@@ -8147,6 +8352,30 @@
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
+      <c r="B43" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="44">
+        <v>1</v>
+      </c>
+      <c r="E43" s="44">
+        <v>1</v>
+      </c>
+      <c r="F43" s="44">
+        <v>1</v>
+      </c>
+      <c r="G43" s="44">
+        <v>1</v>
+      </c>
+      <c r="H43" s="44">
+        <v>0</v>
+      </c>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
       <c r="R43" s="31"/>
       <c r="S43" s="28">
         <v>1155</v>
@@ -8213,6 +8442,30 @@
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2">
+        <v>1</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1</v>
+      </c>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
       <c r="R44" s="31"/>
       <c r="S44" s="28">
         <v>1158</v>
@@ -8279,6 +8532,16 @@
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" s="31"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
       <c r="R45" s="31"/>
       <c r="S45" s="28">
         <v>1164</v>
@@ -8597,16 +8860,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:P1"/>
+  <mergeCells count="4">
+    <mergeCell ref="B11:P11"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="J12:Q12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>